<commit_message>
Update approvals via Streamlit
</commit_message>
<xml_diff>
--- a/PENDING_APPROVAL_SHEET (19).xlsx
+++ b/PENDING_APPROVAL_SHEET (19).xlsx
@@ -58614,8 +58614,16 @@
       <c r="AF499" t="inlineStr"/>
       <c r="AG499" t="inlineStr"/>
       <c r="AH499" t="inlineStr"/>
-      <c r="AI499" t="inlineStr"/>
-      <c r="AJ499" t="inlineStr"/>
+      <c r="AI499" t="inlineStr">
+        <is>
+          <t>ACCEPTED</t>
+        </is>
+      </c>
+      <c r="AJ499" t="inlineStr">
+        <is>
+          <t>REJECTED</t>
+        </is>
+      </c>
     </row>
     <row r="500">
       <c r="A500" t="inlineStr">
@@ -58734,8 +58742,16 @@
       <c r="AF500" t="inlineStr"/>
       <c r="AG500" t="inlineStr"/>
       <c r="AH500" t="inlineStr"/>
-      <c r="AI500" t="inlineStr"/>
-      <c r="AJ500" t="inlineStr"/>
+      <c r="AI500" t="inlineStr">
+        <is>
+          <t>ACCEPTED</t>
+        </is>
+      </c>
+      <c r="AJ500" t="inlineStr">
+        <is>
+          <t>ACCEPTED</t>
+        </is>
+      </c>
     </row>
     <row r="501">
       <c r="A501" t="inlineStr">
@@ -58854,8 +58870,16 @@
       <c r="AF501" t="inlineStr"/>
       <c r="AG501" t="inlineStr"/>
       <c r="AH501" t="inlineStr"/>
-      <c r="AI501" t="inlineStr"/>
-      <c r="AJ501" t="inlineStr"/>
+      <c r="AI501" t="inlineStr">
+        <is>
+          <t>ACCEPTED</t>
+        </is>
+      </c>
+      <c r="AJ501" t="inlineStr">
+        <is>
+          <t>ACCEPTED</t>
+        </is>
+      </c>
     </row>
     <row r="502">
       <c r="A502" t="inlineStr">
@@ -58974,8 +58998,16 @@
       <c r="AF502" t="inlineStr"/>
       <c r="AG502" t="inlineStr"/>
       <c r="AH502" t="inlineStr"/>
-      <c r="AI502" t="inlineStr"/>
-      <c r="AJ502" t="inlineStr"/>
+      <c r="AI502" t="inlineStr">
+        <is>
+          <t>ACCEPTED</t>
+        </is>
+      </c>
+      <c r="AJ502" t="inlineStr">
+        <is>
+          <t>ACCEPTED</t>
+        </is>
+      </c>
     </row>
     <row r="503">
       <c r="A503" t="inlineStr">
@@ -59094,8 +59126,16 @@
       <c r="AF503" t="inlineStr"/>
       <c r="AG503" t="inlineStr"/>
       <c r="AH503" t="inlineStr"/>
-      <c r="AI503" t="inlineStr"/>
-      <c r="AJ503" t="inlineStr"/>
+      <c r="AI503" t="inlineStr">
+        <is>
+          <t>ACCEPTED</t>
+        </is>
+      </c>
+      <c r="AJ503" t="inlineStr">
+        <is>
+          <t>ACCEPTED</t>
+        </is>
+      </c>
     </row>
     <row r="504">
       <c r="A504" t="inlineStr">
@@ -59214,8 +59254,16 @@
       <c r="AF504" t="inlineStr"/>
       <c r="AG504" t="inlineStr"/>
       <c r="AH504" t="inlineStr"/>
-      <c r="AI504" t="inlineStr"/>
-      <c r="AJ504" t="inlineStr"/>
+      <c r="AI504" t="inlineStr">
+        <is>
+          <t>ACCEPTED</t>
+        </is>
+      </c>
+      <c r="AJ504" t="inlineStr">
+        <is>
+          <t>ACCEPTED</t>
+        </is>
+      </c>
     </row>
     <row r="505">
       <c r="A505" t="inlineStr">
@@ -59334,8 +59382,16 @@
       <c r="AF505" t="inlineStr"/>
       <c r="AG505" t="inlineStr"/>
       <c r="AH505" t="inlineStr"/>
-      <c r="AI505" t="inlineStr"/>
-      <c r="AJ505" t="inlineStr"/>
+      <c r="AI505" t="inlineStr">
+        <is>
+          <t>ACCEPTED</t>
+        </is>
+      </c>
+      <c r="AJ505" t="inlineStr">
+        <is>
+          <t>ACCEPTED</t>
+        </is>
+      </c>
     </row>
     <row r="506">
       <c r="A506" t="inlineStr">
@@ -59454,8 +59510,16 @@
       <c r="AF506" t="inlineStr"/>
       <c r="AG506" t="inlineStr"/>
       <c r="AH506" t="inlineStr"/>
-      <c r="AI506" t="inlineStr"/>
-      <c r="AJ506" t="inlineStr"/>
+      <c r="AI506" t="inlineStr">
+        <is>
+          <t>ACCEPTED</t>
+        </is>
+      </c>
+      <c r="AJ506" t="inlineStr">
+        <is>
+          <t>ACCEPTED</t>
+        </is>
+      </c>
     </row>
     <row r="507">
       <c r="A507" t="inlineStr">
@@ -59574,7 +59638,11 @@
       <c r="AF507" t="inlineStr"/>
       <c r="AG507" t="inlineStr"/>
       <c r="AH507" t="inlineStr"/>
-      <c r="AI507" t="inlineStr"/>
+      <c r="AI507" t="inlineStr">
+        <is>
+          <t>ACCEPTED</t>
+        </is>
+      </c>
       <c r="AJ507" t="inlineStr"/>
     </row>
     <row r="508">
@@ -59694,7 +59762,11 @@
       <c r="AF508" t="inlineStr"/>
       <c r="AG508" t="inlineStr"/>
       <c r="AH508" t="inlineStr"/>
-      <c r="AI508" t="inlineStr"/>
+      <c r="AI508" t="inlineStr">
+        <is>
+          <t>ACCEPTED</t>
+        </is>
+      </c>
       <c r="AJ508" t="inlineStr"/>
     </row>
     <row r="509">
@@ -59814,7 +59886,11 @@
       <c r="AF509" t="inlineStr"/>
       <c r="AG509" t="inlineStr"/>
       <c r="AH509" t="inlineStr"/>
-      <c r="AI509" t="inlineStr"/>
+      <c r="AI509" t="inlineStr">
+        <is>
+          <t>ACCEPTED</t>
+        </is>
+      </c>
       <c r="AJ509" t="inlineStr"/>
     </row>
     <row r="510">
@@ -59934,8 +60010,16 @@
       <c r="AF510" t="inlineStr"/>
       <c r="AG510" t="inlineStr"/>
       <c r="AH510" t="inlineStr"/>
-      <c r="AI510" t="inlineStr"/>
-      <c r="AJ510" t="inlineStr"/>
+      <c r="AI510" t="inlineStr">
+        <is>
+          <t>ACCEPTED</t>
+        </is>
+      </c>
+      <c r="AJ510" t="inlineStr">
+        <is>
+          <t>ACCEPTED</t>
+        </is>
+      </c>
     </row>
     <row r="511">
       <c r="A511" t="inlineStr">
@@ -60054,8 +60138,16 @@
       <c r="AF511" t="inlineStr"/>
       <c r="AG511" t="inlineStr"/>
       <c r="AH511" t="inlineStr"/>
-      <c r="AI511" t="inlineStr"/>
-      <c r="AJ511" t="inlineStr"/>
+      <c r="AI511" t="inlineStr">
+        <is>
+          <t>ACCEPTED</t>
+        </is>
+      </c>
+      <c r="AJ511" t="inlineStr">
+        <is>
+          <t>REJECTED</t>
+        </is>
+      </c>
     </row>
     <row r="512">
       <c r="A512" t="inlineStr">
@@ -60174,7 +60266,11 @@
       <c r="AF512" t="inlineStr"/>
       <c r="AG512" t="inlineStr"/>
       <c r="AH512" t="inlineStr"/>
-      <c r="AI512" t="inlineStr"/>
+      <c r="AI512" t="inlineStr">
+        <is>
+          <t>REJECTED</t>
+        </is>
+      </c>
       <c r="AJ512" t="inlineStr"/>
     </row>
     <row r="513">
@@ -60294,7 +60390,11 @@
       <c r="AF513" t="inlineStr"/>
       <c r="AG513" t="inlineStr"/>
       <c r="AH513" t="inlineStr"/>
-      <c r="AI513" t="inlineStr"/>
+      <c r="AI513" t="inlineStr">
+        <is>
+          <t>ACCEPTED</t>
+        </is>
+      </c>
       <c r="AJ513" t="inlineStr"/>
     </row>
     <row r="514">
@@ -60416,7 +60516,7 @@
       <c r="AH514" t="inlineStr"/>
       <c r="AI514" t="inlineStr">
         <is>
-          <t>ACCEPTED</t>
+          <t>REJECTED</t>
         </is>
       </c>
       <c r="AJ514" t="inlineStr"/>
@@ -60540,7 +60640,7 @@
       <c r="AH515" t="inlineStr"/>
       <c r="AI515" t="inlineStr">
         <is>
-          <t>ACCEPTED</t>
+          <t>REJECTED</t>
         </is>
       </c>
       <c r="AJ515" t="inlineStr"/>
@@ -60664,7 +60764,7 @@
       <c r="AH516" t="inlineStr"/>
       <c r="AI516" t="inlineStr">
         <is>
-          <t>ACCEPTED</t>
+          <t>REJECTED</t>
         </is>
       </c>
       <c r="AJ516" t="inlineStr"/>

</xml_diff>